<commit_message>
update api_map.xlsx, added note, tags
</commit_message>
<xml_diff>
--- a/src/main/resources/api_map.xlsx
+++ b/src/main/resources/api_map.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>URL_Path</t>
   </si>
@@ -61,6 +61,45 @@
   </si>
   <si>
     <t>получить блокнот</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>получить заметку</t>
+  </si>
+  <si>
+    <t>удалить заметку</t>
+  </si>
+  <si>
+    <t>/{userId}/{noteId}</t>
+  </si>
+  <si>
+    <t>получить заметки</t>
+  </si>
+  <si>
+    <t>получить тэг</t>
+  </si>
+  <si>
+    <t>удалить тэг</t>
+  </si>
+  <si>
+    <t>найти тэг</t>
+  </si>
+  <si>
+    <t>/{usedId}/{tagId}</t>
+  </si>
+  <si>
+    <t>/{usedId}</t>
+  </si>
+  <si>
+    <t>/{userId}/{notebookId}/{noteId}</t>
+  </si>
+  <si>
+    <t>получить  тэги заметки</t>
   </si>
 </sst>
 </file>
@@ -891,18 +930,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -924,7 +963,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -973,6 +1012,104 @@
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>